<commit_message>
Add alias in excel
</commit_message>
<xml_diff>
--- a/rehearsalbpstat.xlsx
+++ b/rehearsalbpstat.xlsx
@@ -16,324 +16,450 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>Block Producer</t>
   </si>
   <si>
+    <t>Alias</t>
+  </si>
+  <si>
     <t>Number of Productions</t>
   </si>
   <si>
     <t>Total Number of Blocks</t>
   </si>
   <si>
+    <t>io15npzu93ug8r3zdeysppnyrcdu2xssz0lcam9l9</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>65809</t>
+  </si>
+  <si>
+    <t>io1xj0u5n20tsqwxh5a3xdtmzuz9wasft0pqjrq8t</t>
+  </si>
+  <si>
+    <t>thebottoken</t>
+  </si>
+  <si>
+    <t>1427</t>
+  </si>
+  <si>
+    <t>io1kr8c6krd7dhxaaqwdkr6erqgu4z0scug3drgja</t>
+  </si>
+  <si>
+    <t>droute</t>
+  </si>
+  <si>
+    <t>1088</t>
+  </si>
+  <si>
+    <t>io17dm3tq9ezgs2uvwrqu8e004l5nqq33jm46r0mg</t>
+  </si>
+  <si>
+    <t>iotexunion</t>
+  </si>
+  <si>
+    <t>1055</t>
+  </si>
+  <si>
+    <t>io12yxdwewry70gr9fs6fphyfaky9c7gurmzk8f4f</t>
+  </si>
+  <si>
+    <t>rosemary11</t>
+  </si>
+  <si>
+    <t>525</t>
+  </si>
+  <si>
+    <t>io1f0rh94m3ctkwep3rlsswwq5vxwlntx4s574l3q</t>
+  </si>
+  <si>
+    <t>yvalidator</t>
+  </si>
+  <si>
+    <t>1411</t>
+  </si>
+  <si>
+    <t>io1wv5m0xyermvr2n0wjx2cjsqwyk863drdl5qfyn</t>
+  </si>
+  <si>
+    <t>rosemary13</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>io1ar5l5s268rtgzshltnqv88mua06ucm58dx678y</t>
+  </si>
+  <si>
+    <t>rosemary</t>
+  </si>
+  <si>
+    <t>1875</t>
+  </si>
+  <si>
+    <t>io1x9kjkr0qv2fa7j4t2as8lrj223xxsqt4tl7xp7</t>
+  </si>
+  <si>
+    <t>rosemary1</t>
+  </si>
+  <si>
+    <t>1968</t>
+  </si>
+  <si>
+    <t>io12wc9ra4la98yay4cqdav5mwxxuzwpt6hk23n3z</t>
+  </si>
+  <si>
+    <t>iotexmainet</t>
+  </si>
+  <si>
+    <t>1650</t>
+  </si>
+  <si>
+    <t>io1sd5t5dwxrk2t50z8yl86n6ht8c99umt4u6rknl</t>
+  </si>
+  <si>
+    <t>hashbuy</t>
+  </si>
+  <si>
+    <t>1729</t>
+  </si>
+  <si>
+    <t>io1n3llm0zzlles6pvpzugzajyzyjehztztxf2rff</t>
+  </si>
+  <si>
+    <t>ratels</t>
+  </si>
+  <si>
+    <t>1099</t>
+  </si>
+  <si>
+    <t>io1v0q5g2f8z6l3v25krl677chdx7g5pwt9kvqfpc</t>
+  </si>
+  <si>
+    <t>419</t>
+  </si>
+  <si>
+    <t>io1gh7xfrsnj6p5uqgjpk9xq6jg9na28aewgp7a9v</t>
+  </si>
+  <si>
+    <t>315</t>
+  </si>
+  <si>
+    <t>io1ddjluttkzljqfgdtcz9eu3r3s832umy7ylx0ts</t>
+  </si>
+  <si>
+    <t>longz</t>
+  </si>
+  <si>
+    <t>1639</t>
+  </si>
+  <si>
+    <t>io1e3w03ulnrsxth2g0rgsq6v406fhdccsgfq3hz7</t>
+  </si>
+  <si>
+    <t>iotask</t>
+  </si>
+  <si>
+    <t>io1we5gqn4xeak9ycnu4l9lv0qfq3euapymnzffx6</t>
+  </si>
+  <si>
+    <t>coingecko</t>
+  </si>
+  <si>
+    <t>1599</t>
+  </si>
+  <si>
+    <t>io1c3r4th3zrk4uhv83a9gr4gvn3y6pzaj6mc84ea</t>
+  </si>
+  <si>
+    <t>rosemary6</t>
+  </si>
+  <si>
+    <t>1384</t>
+  </si>
+  <si>
+    <t>io1z7mjef7w528nasnsafan0rp6yuvkvq405l6r8j</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>io108h7sa5sap44e244hz649zyk5y4rqzsvnpzxh5</t>
+  </si>
+  <si>
+    <t>royalland</t>
+  </si>
+  <si>
+    <t>1557</t>
+  </si>
+  <si>
+    <t>io1vtm2zgn830pn6auc2cvnchgwdaefa9gr4z0s86</t>
+  </si>
+  <si>
+    <t>rosemary4</t>
+  </si>
+  <si>
+    <t>1812</t>
+  </si>
+  <si>
+    <t>io10reczcaelglh5xmkay65h9vw3e5dp82e8vw0rz</t>
+  </si>
+  <si>
+    <t>metanyx</t>
+  </si>
+  <si>
+    <t>1815</t>
+  </si>
+  <si>
+    <t>io159fv8mu9d5djk8u2t0flgw4yqmt6fg98uqjka8</t>
+  </si>
+  <si>
+    <t>rosemary5</t>
+  </si>
+  <si>
+    <t>2174</t>
+  </si>
+  <si>
+    <t>io1du4eq4f88n4wyc026l3gamjwetlgsg4jz7j884</t>
+  </si>
+  <si>
+    <t>rosemary10</t>
+  </si>
+  <si>
+    <t>583</t>
+  </si>
+  <si>
     <t>io15fqav3tugm96ge7anckx0k4gukz5m4mqf0jpv3</t>
   </si>
   <si>
-    <t>1788</t>
-  </si>
-  <si>
-    <t>58347</t>
-  </si>
-  <si>
-    <t>io108h7sa5sap44e244hz649zyk5y4rqzsvnpzxh5</t>
-  </si>
-  <si>
-    <t>1330</t>
-  </si>
-  <si>
-    <t>io1sd5t5dwxrk2t50z8yl86n6ht8c99umt4u6rknl</t>
-  </si>
-  <si>
-    <t>1509</t>
-  </si>
-  <si>
-    <t>io1n3llm0zzlles6pvpzugzajyzyjehztztxf2rff</t>
-  </si>
-  <si>
-    <t>1009</t>
+    <t>rosemary0</t>
+  </si>
+  <si>
+    <t>2046</t>
+  </si>
+  <si>
+    <t>io1fks575kklxafq4fwjccmz5d3pmq5ynxk5h6h0v</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>io1rfeltdr5wgmhm4rdx9eun3pp68ahm7fq00wcmm</t>
+  </si>
+  <si>
+    <t>pubxpayments</t>
+  </si>
+  <si>
+    <t>838</t>
+  </si>
+  <si>
+    <t>io1fra0fx6akacny9asewt7vyvggqq4rtq3eznccr</t>
+  </si>
+  <si>
+    <t>iotexteam</t>
+  </si>
+  <si>
+    <t>1727</t>
+  </si>
+  <si>
+    <t>io127ftn4ry6wgxdrw4hcd6gdwqlq70ujk98dvtw5</t>
+  </si>
+  <si>
+    <t>rosemary12</t>
+  </si>
+  <si>
+    <t>538</t>
+  </si>
+  <si>
+    <t>io14u5d66rt465ykm7t2847qllj0reml27q30kr75</t>
+  </si>
+  <si>
+    <t>iosg</t>
+  </si>
+  <si>
+    <t>1521</t>
+  </si>
+  <si>
+    <t>io1z4sxtefurklkyrfmmdtjmw4h8csnxlv9747hyd</t>
+  </si>
+  <si>
+    <t>preangle</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>io14vmhs9c75r2ptxdaqrtk0dz7skct30pxmt69d9</t>
+  </si>
+  <si>
+    <t>rosemary7</t>
+  </si>
+  <si>
+    <t>1597</t>
+  </si>
+  <si>
+    <t>io1xsx5n94kg2zv64r7tm8vyz9mh86amfak9ka9xx</t>
+  </si>
+  <si>
+    <t>rosemary3</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>io1et7zkzc76m9twa4gn5xht3urt9mwj05qvdtj66</t>
+  </si>
+  <si>
+    <t>iotxplorerio</t>
+  </si>
+  <si>
+    <t>1759</t>
+  </si>
+  <si>
+    <t>io1zy9q4myp3jezxdsv82z3f865ruamhqm7a6mggh</t>
+  </si>
+  <si>
+    <t>capitalmu</t>
+  </si>
+  <si>
+    <t>io1aqf30kqz5rqh6zn82c00j684p2h2t5cg30wm8t</t>
+  </si>
+  <si>
+    <t>keysiotex</t>
+  </si>
+  <si>
+    <t>1647</t>
+  </si>
+  <si>
+    <t>io1jafqlvntcxgyp6e0uxctt3tljzc3vyv5hg4ukh</t>
+  </si>
+  <si>
+    <t>io13v3dhwds82hg0uc9l4puer00k93qagdh62j0mz</t>
+  </si>
+  <si>
+    <t>wannodes</t>
+  </si>
+  <si>
+    <t>1813</t>
+  </si>
+  <si>
+    <t>io1nf0rvzgq3tqym6n3trttsrt7d4gqqsmqfzy0da</t>
+  </si>
+  <si>
+    <t>iotexlab</t>
+  </si>
+  <si>
+    <t>1635</t>
+  </si>
+  <si>
+    <t>io1qqaswtu7rcevahucpfxc0zxx088pylwtxnkrrl</t>
+  </si>
+  <si>
+    <t>cpc</t>
+  </si>
+  <si>
+    <t>io1qnec80ark9shjc6uzk45dhm8s50dpc27sjuver</t>
+  </si>
+  <si>
+    <t>gamefantasy</t>
+  </si>
+  <si>
+    <t>1179</t>
+  </si>
+  <si>
+    <t>io1vlsmjs87jlk93624nppccfn24nk9nplu9uhu53</t>
+  </si>
+  <si>
+    <t>cobo</t>
+  </si>
+  <si>
+    <t>1323</t>
+  </si>
+  <si>
+    <t>io1wl83n3up9w8nedf30lnyxzple0gu5pme0dyrds</t>
+  </si>
+  <si>
+    <t>whales</t>
+  </si>
+  <si>
+    <t>1629</t>
+  </si>
+  <si>
+    <t>io17cmrextyfeu4gddwd89g5qncedsnc553dhz7xa</t>
+  </si>
+  <si>
+    <t>infstones</t>
+  </si>
+  <si>
+    <t>1404</t>
   </si>
   <si>
     <t>io1nyjs526mnqcsx4twa7nptkg08eclsw5c2dywp4</t>
   </si>
   <si>
-    <t>345</t>
-  </si>
-  <si>
-    <t>io127ftn4ry6wgxdrw4hcd6gdwqlq70ujk98dvtw5</t>
-  </si>
-  <si>
-    <t>526</t>
-  </si>
-  <si>
-    <t>io1x9kjkr0qv2fa7j4t2as8lrj223xxsqt4tl7xp7</t>
-  </si>
-  <si>
-    <t>1705</t>
-  </si>
-  <si>
-    <t>io1kr8c6krd7dhxaaqwdkr6erqgu4z0scug3drgja</t>
-  </si>
-  <si>
-    <t>841</t>
-  </si>
-  <si>
-    <t>io14vmhs9c75r2ptxdaqrtk0dz7skct30pxmt69d9</t>
-  </si>
-  <si>
-    <t>1567</t>
+    <t>360</t>
+  </si>
+  <si>
+    <t>io1xsdegzr2hdj5sv5ad4nr0yfgpsd98e40u6svem</t>
+  </si>
+  <si>
+    <t>390</t>
+  </si>
+  <si>
+    <t>io1scs89jur7qklzh5vfrmha3c40u8yajjx6kvzg9</t>
+  </si>
+  <si>
+    <t>io1u5ff879gg2dw9vfpxr2tsmuaz07e2rea6gvl7s</t>
+  </si>
+  <si>
+    <t>rosemary9</t>
+  </si>
+  <si>
+    <t>839</t>
+  </si>
+  <si>
+    <t>io1kugyfdkdss7acy0y9x8fmfjd5qyxfcye3gxt99</t>
+  </si>
+  <si>
+    <t>consensusnet</t>
+  </si>
+  <si>
+    <t>1726</t>
+  </si>
+  <si>
+    <t>io1gfq9el2gnguus64ex3hu8ajd6e4yzk3f9cz5vx</t>
+  </si>
+  <si>
+    <t>laomao</t>
+  </si>
+  <si>
+    <t>567</t>
+  </si>
+  <si>
+    <t>io1cup9k8hl8fp40vrj29ex8djc346780dk223end</t>
   </si>
   <si>
     <t>io1gf08snppu2a2wfd50pjas2j6q2kcxjzqph3pep</t>
   </si>
   <si>
+    <t>rosemary8</t>
+  </si>
+  <si>
     <t>1048</t>
   </si>
   <si>
-    <t>io1wl83n3up9w8nedf30lnyxzple0gu5pme0dyrds</t>
-  </si>
-  <si>
-    <t>1427</t>
-  </si>
-  <si>
-    <t>io1u5ff879gg2dw9vfpxr2tsmuaz07e2rea6gvl7s</t>
-  </si>
-  <si>
-    <t>839</t>
-  </si>
-  <si>
-    <t>io17cmrextyfeu4gddwd89g5qncedsnc553dhz7xa</t>
-  </si>
-  <si>
-    <t>1143</t>
-  </si>
-  <si>
-    <t>io1gh7xfrsnj6p5uqgjpk9xq6jg9na28aewgp7a9v</t>
-  </si>
-  <si>
-    <t>272</t>
-  </si>
-  <si>
-    <t>io1z4sxtefurklkyrfmmdtjmw4h8csnxlv9747hyd</t>
-  </si>
-  <si>
-    <t>1589</t>
-  </si>
-  <si>
-    <t>io1rfeltdr5wgmhm4rdx9eun3pp68ahm7fq00wcmm</t>
-  </si>
-  <si>
-    <t>817</t>
-  </si>
-  <si>
-    <t>io1du4eq4f88n4wyc026l3gamjwetlgsg4jz7j884</t>
-  </si>
-  <si>
-    <t>568</t>
-  </si>
-  <si>
-    <t>io1c3r4th3zrk4uhv83a9gr4gvn3y6pzaj6mc84ea</t>
-  </si>
-  <si>
-    <t>1384</t>
-  </si>
-  <si>
-    <t>io1cup9k8hl8fp40vrj29ex8djc346780dk223end</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
     <t>io1lm85qfm24eqrc042spnplac9ran28thuh5048n</t>
   </si>
   <si>
-    <t>1485</t>
-  </si>
-  <si>
-    <t>io14u5d66rt465ykm7t2847qllj0reml27q30kr75</t>
-  </si>
-  <si>
-    <t>1323</t>
-  </si>
-  <si>
-    <t>io13v3dhwds82hg0uc9l4puer00k93qagdh62j0mz</t>
-  </si>
-  <si>
-    <t>1588</t>
-  </si>
-  <si>
-    <t>io1e3w03ulnrsxth2g0rgsq6v406fhdccsgfq3hz7</t>
-  </si>
-  <si>
-    <t>1547</t>
-  </si>
-  <si>
-    <t>io1f0rh94m3ctkwep3rlsswwq5vxwlntx4s574l3q</t>
-  </si>
-  <si>
-    <t>1238</t>
-  </si>
-  <si>
-    <t>io1jafqlvntcxgyp6e0uxctt3tljzc3vyv5hg4ukh</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>io12yxdwewry70gr9fs6fphyfaky9c7gurmzk8f4f</t>
-  </si>
-  <si>
-    <t>525</t>
-  </si>
-  <si>
-    <t>io12wc9ra4la98yay4cqdav5mwxxuzwpt6hk23n3z</t>
-  </si>
-  <si>
-    <t>1471</t>
-  </si>
-  <si>
-    <t>io1zy9q4myp3jezxdsv82z3f865ruamhqm7a6mggh</t>
-  </si>
-  <si>
-    <t>1538</t>
-  </si>
-  <si>
-    <t>io1ddjluttkzljqfgdtcz9eu3r3s832umy7ylx0ts</t>
-  </si>
-  <si>
-    <t>1477</t>
-  </si>
-  <si>
-    <t>io1gfq9el2gnguus64ex3hu8ajd6e4yzk3f9cz5vx</t>
-  </si>
-  <si>
-    <t>362</t>
-  </si>
-  <si>
-    <t>io1xsx5n94kg2zv64r7tm8vyz9mh86amfak9ka9xx</t>
-  </si>
-  <si>
-    <t>1794</t>
-  </si>
-  <si>
-    <t>io1kugyfdkdss7acy0y9x8fmfjd5qyxfcye3gxt99</t>
-  </si>
-  <si>
-    <t>1502</t>
-  </si>
-  <si>
-    <t>io1et7zkzc76m9twa4gn5xht3urt9mwj05qvdtj66</t>
-  </si>
-  <si>
-    <t>1440</t>
-  </si>
-  <si>
-    <t>io1v0q5g2f8z6l3v25krl677chdx7g5pwt9kvqfpc</t>
-  </si>
-  <si>
-    <t>404</t>
-  </si>
-  <si>
-    <t>io1scs89jur7qklzh5vfrmha3c40u8yajjx6kvzg9</t>
-  </si>
-  <si>
-    <t>io1qnec80ark9shjc6uzk45dhm8s50dpc27sjuver</t>
-  </si>
-  <si>
-    <t>981</t>
-  </si>
-  <si>
-    <t>io1wv5m0xyermvr2n0wjx2cjsqwyk863drdl5qfyn</t>
-  </si>
-  <si>
-    <t>390</t>
-  </si>
-  <si>
-    <t>io15npzu93ug8r3zdeysppnyrcdu2xssz0lcam9l9</t>
-  </si>
-  <si>
-    <t>389</t>
-  </si>
-  <si>
-    <t>io1we5gqn4xeak9ycnu4l9lv0qfq3euapymnzffx6</t>
-  </si>
-  <si>
-    <t>1336</t>
-  </si>
-  <si>
-    <t>io1ar5l5s268rtgzshltnqv88mua06ucm58dx678y</t>
-  </si>
-  <si>
-    <t>1681</t>
-  </si>
-  <si>
-    <t>io1aqf30kqz5rqh6zn82c00j684p2h2t5cg30wm8t</t>
-  </si>
-  <si>
-    <t>1436</t>
-  </si>
-  <si>
-    <t>io1qqaswtu7rcevahucpfxc0zxx088pylwtxnkrrl</t>
-  </si>
-  <si>
-    <t>1472</t>
-  </si>
-  <si>
-    <t>io1vlsmjs87jlk93624nppccfn24nk9nplu9uhu53</t>
-  </si>
-  <si>
-    <t>1203</t>
-  </si>
-  <si>
-    <t>io1nf0rvzgq3tqym6n3trttsrt7d4gqqsmqfzy0da</t>
-  </si>
-  <si>
-    <t>1468</t>
-  </si>
-  <si>
-    <t>io17dm3tq9ezgs2uvwrqu8e004l5nqq33jm46r0mg</t>
-  </si>
-  <si>
-    <t>795</t>
-  </si>
-  <si>
-    <t>io1vtm2zgn830pn6auc2cvnchgwdaefa9gr4z0s86</t>
-  </si>
-  <si>
-    <t>io1fra0fx6akacny9asewt7vyvggqq4rtq3eznccr</t>
-  </si>
-  <si>
-    <t>1546</t>
-  </si>
-  <si>
-    <t>io1xj0u5n20tsqwxh5a3xdtmzuz9wasft0pqjrq8t</t>
-  </si>
-  <si>
-    <t>1316</t>
-  </si>
-  <si>
-    <t>io1z7mjef7w528nasnsafan0rp6yuvkvq405l6r8j</t>
-  </si>
-  <si>
-    <t>315</t>
-  </si>
-  <si>
-    <t>io1fks575kklxafq4fwjccmz5d3pmq5ynxk5h6h0v</t>
-  </si>
-  <si>
-    <t>io10reczcaelglh5xmkay65h9vw3e5dp82e8vw0rz</t>
-  </si>
-  <si>
-    <t>1488</t>
-  </si>
-  <si>
-    <t>io1xsdegzr2hdj5sv5ad4nr0yfgpsd98e40u6svem</t>
-  </si>
-  <si>
-    <t>io159fv8mu9d5djk8u2t0flgw4yqmt6fg98uqjka8</t>
-  </si>
-  <si>
-    <t>1891</t>
+    <t>iotexgeeks</t>
+  </si>
+  <si>
+    <t>1616</t>
   </si>
 </sst>
 </file>
@@ -703,7 +829,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -714,6 +840,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40" customWidth="true"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40" customWidth="true"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40" customWidth="true"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -726,588 +853,730 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="1" t="s"/>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s"/>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s"/>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s"/>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>68</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B27" s="1" t="s"/>
       <c r="C27" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>5</v>
+        <v>79</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>5</v>
+        <v>82</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>5</v>
+        <v>88</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>5</v>
+        <v>94</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>5</v>
+        <v>97</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>5</v>
+        <v>105</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B38" s="1" t="s"/>
       <c r="C38" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>5</v>
+        <v>109</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>5</v>
+        <v>112</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>5</v>
+        <v>117</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>5</v>
+        <v>120</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>5</v>
+        <v>123</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>5</v>
+        <v>126</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B46" s="1" t="s"/>
       <c r="C46" s="1" t="s">
-        <v>5</v>
+        <v>128</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="B47" s="1" t="s"/>
       <c r="C47" s="1" t="s">
-        <v>5</v>
+        <v>130</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>95</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s"/>
       <c r="C48" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>5</v>
+        <v>134</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>5</v>
+        <v>137</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>5</v>
+        <v>140</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B52" s="1" t="s"/>
       <c r="C52" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>5</v>
+        <v>144</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>5</v>
+        <v>147</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>